<commit_message>
Cierre semana y ciclico con nuevo cambio
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/inventariociclico.xlsx
+++ b/public/application/files/jasper/templates/inventariociclico.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27020" yWindow="0" windowWidth="25500" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="3840" windowWidth="25360" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Inventario cíclico</t>
+  </si>
+  <si>
+    <t>{col:diecisiete}</t>
+  </si>
+  <si>
+    <t>{col:dieciocho}</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,18 +205,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -221,8 +223,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -237,6 +242,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -251,6 +257,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,174 +600,188 @@
     <col min="17" max="17" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" ht="28">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="28">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" ht="28">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="1"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:18" ht="28">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:19" ht="28">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="1"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="18">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:19" ht="18">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+    <row r="5" spans="1:19">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:19">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q6" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A5:S5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>